<commit_message>
add train or test feature data
</commit_message>
<xml_diff>
--- a/2021/data/cryptic_pocket_apo.xlsx
+++ b/2021/data/cryptic_pocket_apo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkumada/Documents/class/2021/work/research/2021/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B027DCDD-3103-1443-938F-4F11B4AEE38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8D649DF3-7076-5F43-AC5C-085F50C34F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{BF094E97-5A57-DA4C-8161-3E6398E8ED91}"/>
+    <workbookView xWindow="2200" yWindow="860" windowWidth="28800" windowHeight="16520" xr2:uid="{BF094E97-5A57-DA4C-8161-3E6398E8ED91}"/>
   </bookViews>
   <sheets>
     <sheet name="cryptic_pocket_apo_train" sheetId="6" r:id="rId1"/>
@@ -16918,7 +16918,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" sqref="A1:V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>